<commit_message>
Corrigindo 1.3 - Remoção
</commit_message>
<xml_diff>
--- a/Estoque.xlsx
+++ b/Estoque.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -551,26 +551,9 @@
         <v>G</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>K</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Relogio</v>
-      </c>
-      <c r="C11" t="str">
-        <v>23</v>
-      </c>
-      <c r="D11" t="str">
-        <v>157.98</v>
-      </c>
-      <c r="E11" t="str">
-        <v>44mm</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>